<commit_message>
added oscilloscope data from 19 june
</commit_message>
<xml_diff>
--- a/Laser_Characterisation/Laser_Characterisation_data.xlsx
+++ b/Laser_Characterisation/Laser_Characterisation_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d45d4c4f22f2f2b/UNIVERSITY/MASTERS Quantum Information Science/Spring DTU/Experimental_Techniques/NV_PROJECT/Laser_Characterisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E8CC6C2-CE5E-C046-BDAF-D848CB0FF351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{4E8CC6C2-CE5E-C046-BDAF-D848CB0FF351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82C92947-328D-D845-900E-E0EBC2CCA5C8}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{D920A05D-74BA-5542-BF5D-4836D706F13B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>Current mA</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>mW</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -2092,6 +2101,150 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>810460</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>463063</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE4DEBBA-704E-A61A-299F-F5A96C04ECB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="810460" y="6667500"/>
+          <a:ext cx="4732603" cy="3314700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63655E05-6295-9ABA-2EB5-30AE5778DDAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2641600" y="8191500"/>
+          <a:ext cx="0" cy="1231900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C72E928-8A2B-644B-8E06-1ED4D6D94789}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1638300" y="8775700"/>
+          <a:ext cx="1371600" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2412,10 +2565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090D7CAC-620C-7D43-BF6D-BA90B3847BCC}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2851,7 +3004,10 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
       <c r="H23" t="str">
         <f>I2</f>
         <v>Current mA</v>
@@ -2860,8 +3016,11 @@
         <f>J2</f>
         <v>Voltage mV</v>
       </c>
+      <c r="J23" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
       <c r="H24">
         <f>I8</f>
         <v>199.99</v>
@@ -2870,8 +3029,12 @@
         <f>J8</f>
         <v>0.248</v>
       </c>
+      <c r="J24">
+        <f>I24*I24/50</f>
+        <v>1.2300799999999999E-3</v>
+      </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
       <c r="H25">
         <f t="shared" ref="H25:I25" si="4">I9</f>
         <v>225.15</v>
@@ -2880,58 +3043,82 @@
         <f t="shared" si="4"/>
         <v>0.67400000000000004</v>
       </c>
+      <c r="J25">
+        <f t="shared" ref="J25:J31" si="5">I25*I25/50</f>
+        <v>9.0855200000000014E-3</v>
+      </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
       <c r="H26">
-        <f t="shared" ref="H26:I26" si="5">I10</f>
+        <f t="shared" ref="H26:I26" si="6">I10</f>
         <v>250.01</v>
       </c>
       <c r="I26">
+        <f t="shared" si="6"/>
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="5"/>
-        <v>1.4350000000000001</v>
+        <v>4.1184499999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
       <c r="H27">
-        <f t="shared" ref="H27:I27" si="6">I11</f>
+        <f t="shared" ref="H27:I27" si="7">I11</f>
         <v>274.77999999999997</v>
       </c>
       <c r="I27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.637</v>
       </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>0.13907538</v>
+      </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
       <c r="H28">
-        <f t="shared" ref="H28:I28" si="7">I12</f>
+        <f t="shared" ref="H28:I28" si="8">I12</f>
         <v>300.05</v>
       </c>
       <c r="I28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.964</v>
       </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>0.31426591999999998</v>
+      </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
       <c r="H29">
-        <f t="shared" ref="H29:I29" si="8">I13</f>
+        <f t="shared" ref="H29:I29" si="9">I13</f>
         <v>324.8</v>
       </c>
       <c r="I29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4210000000000003</v>
       </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>0.58774482000000006</v>
+      </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
       <c r="H30">
-        <f t="shared" ref="H30:I30" si="9">I14</f>
+        <f t="shared" ref="H30:I30" si="10">I14</f>
         <v>350.05</v>
       </c>
       <c r="I30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.1760000000000002</v>
       </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>0.76285952000000012</v>
+      </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
       <c r="H31">
         <f>I15</f>
         <v>375.01</v>
@@ -2939,6 +3126,15 @@
       <c r="I31">
         <f>J15</f>
         <v>8.2360000000000007</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="5"/>
+        <v>1.3566339200000002</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>